<commit_message>
business internet prepaid & postpaid added
</commit_message>
<xml_diff>
--- a/public/sample-format/business-internet-product.xlsx
+++ b/public/sample-format/business-internet-product.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp2\htdocs\bl_cms\public\sample-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80BB4C5-1E48-4E44-BC79-E98F2D3CB53C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8F769E-48D5-4BD8-901E-3420D350AFA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Postpaid Offer List" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Postpaid Offer List'!$A$1:$S$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Postpaid Offer List'!$B$1:$T$11</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="163">
   <si>
     <t>Product Code</t>
   </si>
@@ -514,6 +514,15 @@
   </si>
   <si>
     <t>*5000*58#</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Prepaid</t>
+  </si>
+  <si>
+    <t>Postpaid</t>
   </si>
 </sst>
 </file>
@@ -532,12 +541,13 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -760,7 +770,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1159,1466 +1179,1542 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:ALW50"/>
+  <dimension ref="A1:ALX50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:V24"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17.6640625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="29.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20" style="1" customWidth="1"/>
-    <col min="9" max="9" width="24" style="1" customWidth="1"/>
-    <col min="10" max="10" width="18.21875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="11.88671875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="9.33203125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="9.88671875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="14.77734375" style="3" customWidth="1"/>
-    <col min="17" max="17" width="18.44140625" style="2" customWidth="1"/>
-    <col min="18" max="19" width="21.109375" style="1" customWidth="1"/>
-    <col min="20" max="20" width="12.109375" customWidth="1"/>
-    <col min="21" max="21" width="21.44140625" customWidth="1"/>
-    <col min="22" max="22" width="13.5546875" customWidth="1"/>
-    <col min="23" max="23" width="39.6640625" style="1" customWidth="1"/>
-    <col min="24" max="1011" width="9.109375" style="1" customWidth="1"/>
-    <col min="1012" max="1016" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" style="10" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.21875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="29.88671875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20" style="1" customWidth="1"/>
+    <col min="10" max="10" width="24" style="1" customWidth="1"/>
+    <col min="11" max="11" width="18.21875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="11.88671875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="13.33203125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="9.88671875" style="3" customWidth="1"/>
+    <col min="17" max="17" width="14.77734375" style="3" customWidth="1"/>
+    <col min="18" max="18" width="18.44140625" style="2" customWidth="1"/>
+    <col min="19" max="20" width="21.109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="12.109375" customWidth="1"/>
+    <col min="22" max="22" width="21.44140625" customWidth="1"/>
+    <col min="23" max="23" width="13.5546875" customWidth="1"/>
+    <col min="24" max="24" width="39.6640625" style="1" customWidth="1"/>
+    <col min="25" max="1012" width="9.109375" style="1" customWidth="1"/>
+    <col min="1013" max="1017" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:23" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="19"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="F2" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="G2" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="H2" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="I2" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="J2" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="19">
+      <c r="K2" s="19">
         <v>1</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="L2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L2" s="9">
+      <c r="M2" s="9">
         <v>30</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="N2" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="16">
+      <c r="O2" s="16">
         <v>76</v>
       </c>
-      <c r="O2" s="17">
+      <c r="P2" s="17">
         <v>65</v>
       </c>
-      <c r="P2" s="17">
+      <c r="Q2" s="17">
         <v>10.725</v>
       </c>
-      <c r="Q2" s="21" t="s">
+      <c r="R2" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="R2" s="19"/>
       <c r="S2" s="19"/>
-      <c r="T2" s="10" t="s">
+      <c r="T2" s="19"/>
+      <c r="U2" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U2" s="19"/>
       <c r="V2" s="19"/>
-    </row>
-    <row r="3" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="18" t="s">
+      <c r="W2" s="19"/>
+    </row>
+    <row r="3" spans="1:23" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B3" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="G3" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="H3" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="I3" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="J3" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="19">
+      <c r="K3" s="19">
         <v>10</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="L3" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="9">
+      <c r="M3" s="9">
         <v>7</v>
       </c>
-      <c r="M3" s="21" t="s">
+      <c r="N3" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="16">
+      <c r="O3" s="16">
         <v>129</v>
       </c>
-      <c r="O3" s="17">
+      <c r="P3" s="17">
         <v>111</v>
       </c>
-      <c r="P3" s="17">
+      <c r="Q3" s="17">
         <v>18.315000000000001</v>
       </c>
-      <c r="Q3" s="21" t="s">
+      <c r="R3" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="R3" s="19"/>
       <c r="S3" s="19"/>
-      <c r="T3" s="10" t="s">
+      <c r="T3" s="19"/>
+      <c r="U3" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U3" s="19"/>
       <c r="V3" s="19"/>
-    </row>
-    <row r="4" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="18" t="s">
+      <c r="W3" s="19"/>
+    </row>
+    <row r="4" spans="1:23" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="12" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="G4" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="H4" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="I4" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="J4" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="19">
+      <c r="K4" s="19">
         <v>3</v>
       </c>
-      <c r="K4" s="21" t="s">
+      <c r="L4" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L4" s="9">
+      <c r="M4" s="9">
         <v>7</v>
       </c>
-      <c r="M4" s="21" t="s">
+      <c r="N4" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N4" s="16">
+      <c r="O4" s="16">
         <v>99</v>
       </c>
-      <c r="O4" s="17">
+      <c r="P4" s="17">
         <v>85</v>
       </c>
-      <c r="P4" s="17">
+      <c r="Q4" s="17">
         <v>14.025</v>
       </c>
-      <c r="Q4" s="21"/>
-      <c r="R4" s="19"/>
+      <c r="R4" s="21"/>
       <c r="S4" s="19"/>
-      <c r="T4" s="10" t="s">
+      <c r="T4" s="19"/>
+      <c r="U4" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U4" s="19"/>
       <c r="V4" s="19"/>
-    </row>
-    <row r="5" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="18" t="s">
+      <c r="W4" s="19"/>
+    </row>
+    <row r="5" spans="1:23" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="12" t="s">
+      <c r="C5" s="19"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="G5" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="I5" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="J5" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="19">
+      <c r="K5" s="19">
         <v>2</v>
       </c>
-      <c r="K5" s="21" t="s">
+      <c r="L5" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="9">
+      <c r="M5" s="9">
         <v>4</v>
       </c>
-      <c r="M5" s="21" t="s">
+      <c r="N5" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N5" s="16">
+      <c r="O5" s="16">
         <v>49</v>
       </c>
-      <c r="O5" s="17">
+      <c r="P5" s="17">
         <v>42</v>
       </c>
-      <c r="P5" s="17">
+      <c r="Q5" s="17">
         <v>6.9300000000000006</v>
       </c>
-      <c r="Q5" s="21" t="s">
+      <c r="R5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="R5" s="19"/>
       <c r="S5" s="19"/>
-      <c r="T5" s="10" t="s">
+      <c r="T5" s="19"/>
+      <c r="U5" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U5" s="19"/>
       <c r="V5" s="19"/>
-    </row>
-    <row r="6" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="18" t="s">
+      <c r="W5" s="19"/>
+    </row>
+    <row r="6" spans="1:23" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="19"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="G6" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="I6" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="I6" s="19" t="s">
+      <c r="J6" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J6" s="19">
+      <c r="K6" s="19">
         <v>3</v>
       </c>
-      <c r="K6" s="21" t="s">
+      <c r="L6" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="9">
+      <c r="M6" s="9">
         <v>30</v>
       </c>
-      <c r="M6" s="21" t="s">
+      <c r="N6" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N6" s="16">
+      <c r="O6" s="16">
         <v>249</v>
       </c>
-      <c r="O6" s="17">
+      <c r="P6" s="17">
         <v>213.73390557939913</v>
       </c>
-      <c r="P6" s="17">
+      <c r="Q6" s="17">
         <v>35.266094420600858</v>
       </c>
-      <c r="Q6" s="21" t="s">
+      <c r="R6" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="R6" s="19"/>
       <c r="S6" s="19"/>
-      <c r="T6" s="10" t="s">
+      <c r="T6" s="19"/>
+      <c r="U6" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U6" s="19"/>
       <c r="V6" s="19"/>
-    </row>
-    <row r="7" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="18" t="s">
+      <c r="W6" s="19"/>
+    </row>
+    <row r="7" spans="1:23" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="12" t="s">
+      <c r="C7" s="19"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="G7" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="H7" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="I7" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="I7" s="19" t="s">
+      <c r="J7" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J7" s="19">
+      <c r="K7" s="19">
         <v>20</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="L7" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L7" s="9">
+      <c r="M7" s="9">
         <v>7</v>
       </c>
-      <c r="M7" s="21" t="s">
+      <c r="N7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N7" s="16">
+      <c r="O7" s="16">
         <v>199</v>
       </c>
-      <c r="O7" s="17">
+      <c r="P7" s="17">
         <v>171</v>
       </c>
-      <c r="P7" s="17">
+      <c r="Q7" s="17">
         <v>28.215</v>
       </c>
-      <c r="Q7" s="21" t="s">
+      <c r="R7" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="R7" s="19"/>
       <c r="S7" s="19"/>
-      <c r="T7" s="10" t="s">
+      <c r="T7" s="19"/>
+      <c r="U7" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U7" s="19"/>
       <c r="V7" s="19"/>
-    </row>
-    <row r="8" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="18" t="s">
+      <c r="W7" s="19"/>
+    </row>
+    <row r="8" spans="1:23" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="12" t="s">
+      <c r="C8" s="19"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="G8" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="H8" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="I8" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="I8" s="19" t="s">
+      <c r="J8" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J8" s="19">
+      <c r="K8" s="19">
         <v>18</v>
       </c>
-      <c r="K8" s="21" t="s">
+      <c r="L8" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="9">
+      <c r="M8" s="9">
         <v>30</v>
       </c>
-      <c r="M8" s="21" t="s">
+      <c r="N8" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N8" s="16">
+      <c r="O8" s="16">
         <v>499</v>
       </c>
-      <c r="O8" s="17">
+      <c r="P8" s="17">
         <v>428.33</v>
       </c>
-      <c r="P8" s="17">
+      <c r="Q8" s="17">
         <v>70.674450000000007</v>
       </c>
-      <c r="Q8" s="21" t="s">
+      <c r="R8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="R8" s="19"/>
       <c r="S8" s="19"/>
-      <c r="T8" s="10" t="s">
+      <c r="T8" s="19"/>
+      <c r="U8" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U8" s="19"/>
       <c r="V8" s="19"/>
-    </row>
-    <row r="9" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
+      <c r="W8" s="19"/>
+    </row>
+    <row r="9" spans="1:23" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="12" t="s">
+      <c r="C9" s="19"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="G9" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="H9" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="I9" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I9" s="19" t="s">
+      <c r="J9" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="19">
+      <c r="K9" s="19">
         <v>12</v>
       </c>
-      <c r="K9" s="21" t="s">
+      <c r="L9" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L9" s="9">
+      <c r="M9" s="9">
         <v>30</v>
       </c>
-      <c r="M9" s="21" t="s">
+      <c r="N9" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N9" s="16">
+      <c r="O9" s="16">
         <v>399</v>
       </c>
-      <c r="O9" s="17">
+      <c r="P9" s="17">
         <v>342.49</v>
       </c>
-      <c r="P9" s="17">
+      <c r="Q9" s="17">
         <v>56.510850000000005</v>
       </c>
-      <c r="Q9" s="21" t="s">
+      <c r="R9" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="R9" s="19"/>
       <c r="S9" s="19"/>
-      <c r="T9" s="10" t="s">
+      <c r="T9" s="19"/>
+      <c r="U9" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U9" s="19"/>
       <c r="V9" s="19"/>
-    </row>
-    <row r="10" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="18" t="s">
+      <c r="W9" s="19"/>
+    </row>
+    <row r="10" spans="1:23" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B10" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="12" t="s">
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="F10" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="G10" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="H10" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="15" t="s">
+      <c r="I10" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="19" t="s">
+      <c r="J10" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J10" s="19">
+      <c r="K10" s="19">
         <v>1</v>
       </c>
-      <c r="K10" s="21" t="s">
+      <c r="L10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L10" s="11">
+      <c r="M10" s="11">
         <v>4</v>
       </c>
-      <c r="M10" s="21" t="s">
+      <c r="N10" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N10" s="9">
+      <c r="O10" s="9">
         <v>36</v>
       </c>
-      <c r="O10" s="9">
+      <c r="P10" s="9">
         <v>31</v>
       </c>
-      <c r="P10" s="9">
+      <c r="Q10" s="9">
         <v>5.1150000000000002</v>
       </c>
-      <c r="Q10" s="21" t="s">
+      <c r="R10" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="R10" s="19"/>
       <c r="S10" s="19"/>
-      <c r="T10" s="10" t="s">
+      <c r="T10" s="19"/>
+      <c r="U10" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U10" s="19"/>
       <c r="V10" s="19"/>
-    </row>
-    <row r="11" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="18" t="s">
+      <c r="W10" s="19"/>
+    </row>
+    <row r="11" spans="1:23" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="12" t="s">
+      <c r="C11" s="19"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="F11" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="G11" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="H11" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="I11" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="I11" s="19" t="s">
+      <c r="J11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="19">
+      <c r="K11" s="19">
         <v>1.2</v>
       </c>
-      <c r="K11" s="21" t="s">
+      <c r="L11" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L11" s="11">
+      <c r="M11" s="11">
         <v>30</v>
       </c>
-      <c r="M11" s="21" t="s">
+      <c r="N11" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N11" s="9">
+      <c r="O11" s="9">
         <v>119</v>
       </c>
-      <c r="O11" s="9">
+      <c r="P11" s="9">
         <v>102</v>
       </c>
-      <c r="P11" s="9">
+      <c r="Q11" s="9">
         <v>16.830000000000002</v>
       </c>
-      <c r="Q11" s="21" t="s">
+      <c r="R11" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="R11" s="19"/>
       <c r="S11" s="19"/>
-      <c r="T11" s="10" t="s">
+      <c r="T11" s="19"/>
+      <c r="U11" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U11" s="19"/>
       <c r="V11" s="19"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A12" s="18" t="s">
+      <c r="W11" s="19"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="19" t="s">
+      <c r="C12" s="19"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="19" t="s">
+      <c r="F12" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="19" t="s">
+      <c r="G12" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="H12" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="H12" s="19" t="s">
+      <c r="I12" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="I12" s="19" t="s">
+      <c r="J12" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="19">
+      <c r="K12" s="19">
         <v>2</v>
       </c>
-      <c r="K12" s="21" t="s">
+      <c r="L12" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="22">
+      <c r="M12" s="22">
         <v>30</v>
       </c>
-      <c r="M12" s="21" t="s">
+      <c r="N12" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N12" s="22">
+      <c r="O12" s="22">
         <v>209</v>
       </c>
-      <c r="O12" s="22">
+      <c r="P12" s="22">
         <v>179.4</v>
       </c>
-      <c r="P12" s="22">
+      <c r="Q12" s="22">
         <v>29.601000000000003</v>
       </c>
-      <c r="Q12" s="21"/>
-      <c r="R12" s="19"/>
+      <c r="R12" s="21"/>
       <c r="S12" s="19"/>
-      <c r="T12" s="10" t="s">
+      <c r="T12" s="19"/>
+      <c r="U12" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U12" s="19"/>
       <c r="V12" s="19"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
-      <c r="B13" s="19"/>
-      <c r="C13" s="18" t="s">
+      <c r="W12" s="19"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="E13" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="F13" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="G13" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="H13" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19" t="s">
+      <c r="I13" s="19"/>
+      <c r="J13" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J13" s="19">
+      <c r="K13" s="19">
         <v>4</v>
       </c>
-      <c r="K13" s="21" t="s">
+      <c r="L13" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L13" s="22" t="s">
+      <c r="M13" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="M13" s="21" t="s">
+      <c r="N13" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="N13" s="22">
+      <c r="O13" s="22">
         <v>582.5</v>
       </c>
-      <c r="O13" s="22">
+      <c r="P13" s="22">
         <v>500</v>
       </c>
-      <c r="P13" s="22">
+      <c r="Q13" s="22">
         <v>82.5</v>
       </c>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="19"/>
+      <c r="R13" s="21"/>
       <c r="S13" s="19"/>
-      <c r="T13" s="10" t="s">
+      <c r="T13" s="19"/>
+      <c r="U13" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U13" s="19"/>
       <c r="V13" s="19"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="19"/>
-      <c r="C14" s="18" t="s">
+      <c r="W13" s="19"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="E14" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="F14" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="F14" s="19" t="s">
+      <c r="G14" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="H14" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19" t="s">
+      <c r="I14" s="19"/>
+      <c r="J14" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J14" s="19">
+      <c r="K14" s="19">
         <v>8</v>
       </c>
-      <c r="K14" s="21" t="s">
+      <c r="L14" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="22" t="s">
+      <c r="M14" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="M14" s="21" t="s">
+      <c r="N14" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="N14" s="22">
+      <c r="O14" s="22">
         <v>1048.5</v>
       </c>
-      <c r="O14" s="22">
+      <c r="P14" s="22">
         <v>900</v>
       </c>
-      <c r="P14" s="22">
+      <c r="Q14" s="22">
         <v>148.5</v>
       </c>
-      <c r="Q14" s="21"/>
-      <c r="R14" s="19"/>
+      <c r="R14" s="21"/>
       <c r="S14" s="19"/>
-      <c r="T14" s="10" t="s">
+      <c r="T14" s="19"/>
+      <c r="U14" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U14" s="19"/>
       <c r="V14" s="19"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="18" t="s">
+      <c r="W14" s="19"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="E15" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="F15" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="F15" s="19" t="s">
+      <c r="G15" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="H15" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="19"/>
+      <c r="J15" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J15" s="19">
+      <c r="K15" s="19">
         <v>15</v>
       </c>
-      <c r="K15" s="21" t="s">
+      <c r="L15" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L15" s="22" t="s">
+      <c r="M15" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="M15" s="21" t="s">
+      <c r="N15" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="N15" s="22">
+      <c r="O15" s="22">
         <v>1747.5</v>
       </c>
-      <c r="O15" s="22">
+      <c r="P15" s="22">
         <v>1500</v>
       </c>
-      <c r="P15" s="22">
+      <c r="Q15" s="22">
         <v>247.5</v>
       </c>
-      <c r="Q15" s="21"/>
-      <c r="R15" s="19"/>
+      <c r="R15" s="21"/>
       <c r="S15" s="19"/>
-      <c r="T15" s="10" t="s">
+      <c r="T15" s="19"/>
+      <c r="U15" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U15" s="19"/>
       <c r="V15" s="19"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="18" t="s">
+      <c r="W15" s="19"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="23"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="E16" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="F16" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="G16" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="H16" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19" t="s">
+      <c r="I16" s="19"/>
+      <c r="J16" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J16" s="19">
+      <c r="K16" s="19">
         <v>1.5</v>
       </c>
-      <c r="K16" s="21" t="s">
+      <c r="L16" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="22" t="s">
+      <c r="M16" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="M16" s="21" t="s">
+      <c r="N16" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="N16" s="22">
+      <c r="O16" s="22">
         <v>320.375</v>
       </c>
-      <c r="O16" s="22">
+      <c r="P16" s="22">
         <v>275</v>
       </c>
-      <c r="P16" s="22">
+      <c r="Q16" s="22">
         <v>45.375</v>
       </c>
-      <c r="Q16" s="21"/>
-      <c r="R16" s="19"/>
+      <c r="R16" s="21"/>
       <c r="S16" s="19"/>
-      <c r="T16" s="10" t="s">
+      <c r="T16" s="19"/>
+      <c r="U16" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U16" s="19"/>
       <c r="V16" s="19"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="18" t="s">
+      <c r="W16" s="19"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" s="23"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="D17" s="19" t="s">
+      <c r="E17" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="F17" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="F17" s="19" t="s">
+      <c r="G17" s="19" t="s">
         <v>119</v>
       </c>
-      <c r="G17" s="19" t="s">
+      <c r="H17" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19" t="s">
+      <c r="I17" s="19"/>
+      <c r="J17" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J17" s="19">
+      <c r="K17" s="19">
         <v>600</v>
       </c>
-      <c r="K17" s="21" t="s">
+      <c r="L17" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="L17" s="22" t="s">
+      <c r="M17" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="M17" s="21" t="s">
+      <c r="N17" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="N17" s="22">
+      <c r="O17" s="22">
         <v>174.75</v>
       </c>
-      <c r="O17" s="22">
+      <c r="P17" s="22">
         <v>150</v>
       </c>
-      <c r="P17" s="22">
+      <c r="Q17" s="22">
         <v>24.75</v>
       </c>
-      <c r="Q17" s="21"/>
-      <c r="R17" s="19"/>
+      <c r="R17" s="21"/>
       <c r="S17" s="19"/>
-      <c r="T17" s="10" t="s">
+      <c r="T17" s="19"/>
+      <c r="U17" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U17" s="19"/>
       <c r="V17" s="19"/>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="18" t="s">
+      <c r="W17" s="19"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="E18" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="F18" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="F18" s="19" t="s">
+      <c r="G18" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="H18" s="19" t="s">
         <v>126</v>
       </c>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="19"/>
+      <c r="J18" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J18" s="19">
+      <c r="K18" s="19">
         <v>300</v>
       </c>
-      <c r="K18" s="21" t="s">
+      <c r="L18" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="L18" s="22" t="s">
+      <c r="M18" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="M18" s="21" t="s">
+      <c r="N18" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="N18" s="22">
+      <c r="O18" s="22">
         <v>115.33499999999999</v>
       </c>
-      <c r="O18" s="22">
+      <c r="P18" s="22">
         <v>99</v>
       </c>
-      <c r="P18" s="22">
+      <c r="Q18" s="22">
         <v>16.335000000000001</v>
       </c>
-      <c r="Q18" s="21"/>
-      <c r="R18" s="19"/>
+      <c r="R18" s="21"/>
       <c r="S18" s="19"/>
-      <c r="T18" s="10" t="s">
+      <c r="T18" s="19"/>
+      <c r="U18" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U18" s="19"/>
       <c r="V18" s="19"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="18" t="s">
+      <c r="W18" s="19"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="23"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="E19" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="F19" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="G19" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="H19" s="19" t="s">
         <v>131</v>
       </c>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19" t="s">
+      <c r="I19" s="19"/>
+      <c r="J19" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J19" s="19">
+      <c r="K19" s="19">
         <v>1</v>
       </c>
-      <c r="K19" s="21" t="s">
+      <c r="L19" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="22" t="s">
+      <c r="M19" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="M19" s="21" t="s">
+      <c r="N19" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="N19" s="22">
+      <c r="O19" s="22">
         <v>244.65</v>
       </c>
-      <c r="O19" s="22">
+      <c r="P19" s="22">
         <v>210</v>
       </c>
-      <c r="P19" s="22">
+      <c r="Q19" s="22">
         <v>34.65</v>
       </c>
-      <c r="Q19" s="21"/>
-      <c r="R19" s="19"/>
+      <c r="R19" s="21"/>
       <c r="S19" s="19"/>
-      <c r="T19" s="10" t="s">
+      <c r="T19" s="19"/>
+      <c r="U19" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U19" s="19"/>
       <c r="V19" s="19"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A20" s="24" t="s">
+      <c r="W19" s="19"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="B20" s="19"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="19" t="s">
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="F20" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="F20" s="19" t="s">
+      <c r="G20" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="G20" s="19" t="s">
+      <c r="H20" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="H20" s="19" t="s">
+      <c r="I20" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="I20" s="19" t="s">
+      <c r="J20" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J20" s="19">
+      <c r="K20" s="19">
         <v>14</v>
       </c>
-      <c r="K20" s="21" t="s">
+      <c r="L20" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L20" s="22">
+      <c r="M20" s="22">
         <v>7</v>
       </c>
-      <c r="M20" s="21" t="s">
+      <c r="N20" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N20" s="22">
+      <c r="O20" s="22">
         <v>149</v>
       </c>
-      <c r="O20" s="22">
+      <c r="P20" s="22">
         <v>127.89699570815451</v>
       </c>
-      <c r="P20" s="22">
+      <c r="Q20" s="22">
         <v>21.103004291845494</v>
       </c>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="19"/>
+      <c r="R20" s="21"/>
       <c r="S20" s="19"/>
-      <c r="T20" s="10" t="s">
+      <c r="T20" s="19"/>
+      <c r="U20" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U20" s="19"/>
       <c r="V20" s="19"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A21" s="20" t="s">
+      <c r="W20" s="19"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B21" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="19" t="s">
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="F21" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="F21" s="19" t="s">
+      <c r="G21" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="G21" s="19" t="s">
+      <c r="H21" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="H21" s="19" t="s">
+      <c r="I21" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="I21" s="19" t="s">
+      <c r="J21" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J21" s="19">
+      <c r="K21" s="19">
         <v>6</v>
       </c>
-      <c r="K21" s="21" t="s">
+      <c r="L21" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L21" s="22">
+      <c r="M21" s="22">
         <v>30</v>
       </c>
-      <c r="M21" s="21" t="s">
+      <c r="N21" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N21" s="22">
+      <c r="O21" s="22">
         <v>299</v>
       </c>
-      <c r="O21" s="22">
+      <c r="P21" s="22">
         <v>256.65236051502143</v>
       </c>
-      <c r="P21" s="22">
+      <c r="Q21" s="22">
         <v>42.347639484978572</v>
       </c>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="19"/>
+      <c r="R21" s="21"/>
       <c r="S21" s="19"/>
-      <c r="T21" s="10" t="s">
+      <c r="T21" s="19"/>
+      <c r="U21" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U21" s="19"/>
       <c r="V21" s="19"/>
-    </row>
-    <row r="22" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A22" s="25" t="s">
+      <c r="W21" s="19"/>
+    </row>
+    <row r="22" spans="1:23" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="20"/>
-      <c r="D22" s="19" t="s">
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="F22" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="F22" s="19" t="s">
+      <c r="G22" s="19" t="s">
         <v>146</v>
       </c>
-      <c r="G22" s="19" t="s">
+      <c r="H22" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="H22" s="19" t="s">
+      <c r="I22" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="I22" s="19" t="s">
+      <c r="J22" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J22" s="19">
+      <c r="K22" s="19">
         <v>30</v>
       </c>
-      <c r="K22" s="21" t="s">
+      <c r="L22" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L22" s="22">
+      <c r="M22" s="22">
         <v>30</v>
       </c>
-      <c r="M22" s="21" t="s">
+      <c r="N22" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N22" s="22">
+      <c r="O22" s="22">
         <v>699</v>
       </c>
-      <c r="O22" s="22">
+      <c r="P22" s="22">
         <v>600</v>
       </c>
-      <c r="P22" s="22">
+      <c r="Q22" s="22">
         <v>99</v>
       </c>
-      <c r="Q22" s="21"/>
-      <c r="R22" s="19"/>
+      <c r="R22" s="21"/>
       <c r="S22" s="19"/>
-      <c r="T22" s="10" t="s">
+      <c r="T22" s="19"/>
+      <c r="U22" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U22" s="19"/>
       <c r="V22" s="19"/>
-    </row>
-    <row r="23" spans="1:22" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A23" s="25" t="s">
+      <c r="W22" s="19"/>
+    </row>
+    <row r="23" spans="1:23" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B23" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="B23" s="19"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="19" t="s">
+      <c r="C23" s="19"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="F23" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="F23" s="19" t="s">
+      <c r="G23" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="H23" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="H23" s="19" t="s">
+      <c r="I23" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="I23" s="19" t="s">
+      <c r="J23" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J23" s="19">
+      <c r="K23" s="19">
         <v>45</v>
       </c>
-      <c r="K23" s="21" t="s">
+      <c r="L23" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="22">
+      <c r="M23" s="22">
         <v>30</v>
       </c>
-      <c r="M23" s="21" t="s">
+      <c r="N23" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N23" s="22">
+      <c r="O23" s="22">
         <v>999</v>
       </c>
-      <c r="O23" s="22">
+      <c r="P23" s="22">
         <v>857.51072961373393</v>
       </c>
-      <c r="P23" s="22">
+      <c r="Q23" s="22">
         <v>141.48927038626607</v>
       </c>
-      <c r="Q23" s="21"/>
-      <c r="R23" s="19"/>
+      <c r="R23" s="21"/>
       <c r="S23" s="19"/>
-      <c r="T23" s="10" t="s">
+      <c r="T23" s="19"/>
+      <c r="U23" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U23" s="19"/>
       <c r="V23" s="19"/>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A24" s="20" t="s">
+      <c r="W23" s="19"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="B24" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="19" t="s">
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="F24" s="19" t="s">
         <v>157</v>
       </c>
-      <c r="F24" s="19" t="s">
+      <c r="G24" s="19" t="s">
         <v>158</v>
       </c>
-      <c r="G24" s="19" t="s">
+      <c r="H24" s="19" t="s">
         <v>155</v>
       </c>
-      <c r="H24" s="19" t="s">
+      <c r="I24" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="I24" s="19" t="s">
+      <c r="J24" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J24" s="19">
+      <c r="K24" s="19">
         <v>3</v>
       </c>
-      <c r="K24" s="21" t="s">
+      <c r="L24" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="L24" s="22">
+      <c r="M24" s="22">
         <v>4</v>
       </c>
-      <c r="M24" s="21" t="s">
+      <c r="N24" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="N24" s="22">
+      <c r="O24" s="22">
         <v>58</v>
       </c>
-      <c r="O24" s="22">
+      <c r="P24" s="22">
         <v>49.785407725321889</v>
       </c>
-      <c r="P24" s="22">
+      <c r="Q24" s="22">
         <v>8.214592274678111</v>
       </c>
-      <c r="Q24" s="21"/>
-      <c r="R24" s="19"/>
+      <c r="R24" s="21"/>
       <c r="S24" s="19"/>
-      <c r="T24" s="10" t="s">
+      <c r="T24" s="19"/>
+      <c r="U24" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="U24" s="19"/>
       <c r="V24" s="19"/>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="U25" s="1"/>
+      <c r="W24" s="19"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V25" s="1"/>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="U26" s="1"/>
+      <c r="W25" s="1"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V26" s="1"/>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="U27" s="1"/>
+      <c r="W26" s="1"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V27" s="1"/>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="U28" s="1"/>
+      <c r="W27" s="1"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V28" s="1"/>
-    </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="U29" s="1"/>
+      <c r="W28" s="1"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V29" s="1"/>
-    </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="U30" s="1"/>
+      <c r="W29" s="1"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V30" s="1"/>
-    </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="U31" s="1"/>
+      <c r="W30" s="1"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V31" s="1"/>
-    </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="U32" s="1"/>
+      <c r="W31" s="1"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="V32" s="1"/>
-    </row>
-    <row r="33" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U33" s="1"/>
+      <c r="W32" s="1"/>
+    </row>
+    <row r="33" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V33" s="1"/>
-    </row>
-    <row r="34" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U34" s="1"/>
+      <c r="W33" s="1"/>
+    </row>
+    <row r="34" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V34" s="1"/>
-    </row>
-    <row r="35" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U35" s="1"/>
+      <c r="W34" s="1"/>
+    </row>
+    <row r="35" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V35" s="1"/>
-    </row>
-    <row r="36" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U36" s="1"/>
+      <c r="W35" s="1"/>
+    </row>
+    <row r="36" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V36" s="1"/>
-    </row>
-    <row r="37" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U37" s="1"/>
+      <c r="W36" s="1"/>
+    </row>
+    <row r="37" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V37" s="1"/>
-    </row>
-    <row r="38" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U38" s="1"/>
+      <c r="W37" s="1"/>
+    </row>
+    <row r="38" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V38" s="1"/>
-    </row>
-    <row r="39" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U39" s="1"/>
+      <c r="W38" s="1"/>
+    </row>
+    <row r="39" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V39" s="1"/>
-    </row>
-    <row r="40" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U40" s="1"/>
+      <c r="W39" s="1"/>
+    </row>
+    <row r="40" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V40" s="1"/>
-    </row>
-    <row r="41" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U41" s="1"/>
+      <c r="W40" s="1"/>
+    </row>
+    <row r="41" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V41" s="1"/>
-    </row>
-    <row r="42" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U42" s="1"/>
+      <c r="W41" s="1"/>
+    </row>
+    <row r="42" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V42" s="1"/>
-    </row>
-    <row r="43" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U43" s="1"/>
+      <c r="W42" s="1"/>
+    </row>
+    <row r="43" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V43" s="1"/>
-    </row>
-    <row r="44" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U44" s="1"/>
+      <c r="W43" s="1"/>
+    </row>
+    <row r="44" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V44" s="1"/>
-    </row>
-    <row r="45" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U45" s="1"/>
+      <c r="W44" s="1"/>
+    </row>
+    <row r="45" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V45" s="1"/>
-    </row>
-    <row r="46" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U46" s="1"/>
+      <c r="W45" s="1"/>
+    </row>
+    <row r="46" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V46" s="1"/>
-    </row>
-    <row r="47" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U47" s="1"/>
+      <c r="W46" s="1"/>
+    </row>
+    <row r="47" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V47" s="1"/>
-    </row>
-    <row r="48" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U48" s="1"/>
+      <c r="W47" s="1"/>
+    </row>
+    <row r="48" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V48" s="1"/>
-    </row>
-    <row r="49" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U49" s="1"/>
+      <c r="W48" s="1"/>
+    </row>
+    <row r="49" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V49" s="1"/>
-    </row>
-    <row r="50" spans="21:22" x14ac:dyDescent="0.3">
-      <c r="U50" s="1"/>
+      <c r="W49" s="1"/>
+    </row>
+    <row r="50" spans="22:23" x14ac:dyDescent="0.3">
       <c r="V50" s="1"/>
+      <c r="W50" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <conditionalFormatting sqref="B1:C1">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  <autoFilter ref="B1:T11" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <conditionalFormatting sqref="C1:D1">
+    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="duplicateValues" dxfId="1" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>